<commit_message>
correction JUnitbase et TestControlSuivi
</commit_message>
<xml_diff>
--- a/SonarLysaFX/src/test/resources/Suivi_Quality_Gate-JAVATest.xlsx
+++ b/SonarLysaFX/src/test/resources/Suivi_Quality_Gate-JAVATest.xlsx
@@ -8875,10 +8875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T75"/>
+  <dimension ref="A1:T74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8886,36 +8886,49 @@
     <col min="1" max="16384" width="11.42578125" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>290</v>
       </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5" t="s">
+        <v>189</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -8925,10 +8938,8 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5" t="s">
-        <v>189</v>
-      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -8938,8 +8949,10 @@
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -8949,10 +8962,8 @@
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="5" t="s">
-        <v>188</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -8962,8 +8973,10 @@
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="5" t="s">
+        <v>187</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -8973,10 +8986,8 @@
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="5" t="s">
-        <v>187</v>
-      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -8986,8 +8997,10 @@
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="5" t="s">
+        <v>186</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -8995,27 +9008,26 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>291</v>
       </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -9027,7 +9039,7 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -9039,7 +9051,7 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -9051,7 +9063,7 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -9061,157 +9073,145 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="23" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    <row r="22" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>292</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>177</v>
+      <c r="A28" s="11" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
-        <v>171</v>
+      <c r="A34" s="11"/>
+      <c r="B34" s="10" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="10" t="s">
-        <v>169</v>
+      <c r="A36" s="11" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>220</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="75" spans="20:20" x14ac:dyDescent="0.25">
-      <c r="T75" s="2" t="s">
+    <row r="74" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T74" s="2" t="s">
         <v>155</v>
       </c>
     </row>
@@ -9226,7 +9226,7 @@
   <dimension ref="A1:AA105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9408,7 +9408,7 @@
       <c r="V2" s="41"/>
       <c r="W2" s="40">
         <f t="shared" ref="W2:W33" ca="1" si="0">IF(S2 = "", "", IF( V2 = "", TODAY() - S2, V2 - S2 ))</f>
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="X2" s="41">
         <v>43416</v>
@@ -9560,7 +9560,7 @@
       <c r="V4" s="50"/>
       <c r="W4" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X4" s="50">
         <v>43213</v>
@@ -9640,7 +9640,7 @@
       <c r="V5" s="55"/>
       <c r="W5" s="54">
         <f t="shared" ca="1" si="0"/>
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="X5" s="55">
         <v>43171</v>
@@ -9792,7 +9792,7 @@
       <c r="V7" s="64"/>
       <c r="W7" s="63">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X7" s="64">
         <v>43213</v>
@@ -9872,7 +9872,7 @@
       <c r="V8" s="69"/>
       <c r="W8" s="68">
         <f t="shared" ca="1" si="0"/>
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="X8" s="69">
         <v>72686</v>
@@ -9954,7 +9954,7 @@
       <c r="V9" s="74"/>
       <c r="W9" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="X9" s="74">
         <v>72686</v>
@@ -10114,7 +10114,7 @@
       <c r="V11" s="84"/>
       <c r="W11" s="83">
         <f t="shared" ca="1" si="0"/>
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="X11" s="84">
         <v>72686</v>
@@ -10194,7 +10194,7 @@
       <c r="V12" s="89"/>
       <c r="W12" s="88">
         <f t="shared" ca="1" si="0"/>
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="X12" s="89">
         <v>72686</v>
@@ -10274,7 +10274,7 @@
       <c r="V13" s="94"/>
       <c r="W13" s="93">
         <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="X13" s="94">
         <v>43416</v>
@@ -10352,7 +10352,7 @@
       <c r="V14" s="99"/>
       <c r="W14" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X14" s="99">
         <v>43416</v>
@@ -10432,7 +10432,7 @@
       <c r="V15" s="104"/>
       <c r="W15" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="X15" s="104">
         <v>72686</v>
@@ -10512,7 +10512,7 @@
       <c r="V16" s="109"/>
       <c r="W16" s="108">
         <f t="shared" ca="1" si="0"/>
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="X16" s="109">
         <v>72686</v>
@@ -10592,7 +10592,7 @@
       <c r="V17" s="114"/>
       <c r="W17" s="113">
         <f t="shared" ca="1" si="0"/>
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="X17" s="114">
         <v>72686</v>
@@ -10672,7 +10672,7 @@
       <c r="V18" s="119"/>
       <c r="W18" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="X18" s="119">
         <v>43451</v>
@@ -10752,7 +10752,7 @@
       <c r="V19" s="124"/>
       <c r="W19" s="123">
         <f t="shared" ca="1" si="0"/>
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="X19" s="124">
         <v>43416</v>
@@ -10832,7 +10832,7 @@
       <c r="V20" s="129"/>
       <c r="W20" s="128">
         <f t="shared" ca="1" si="0"/>
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="X20" s="129">
         <v>43451</v>
@@ -10910,7 +10910,7 @@
       <c r="V21" s="134"/>
       <c r="W21" s="133">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X21" s="134">
         <v>72686</v>
@@ -10990,7 +10990,7 @@
       <c r="V22" s="139"/>
       <c r="W22" s="138">
         <f t="shared" ca="1" si="0"/>
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="X22" s="139">
         <v>72686</v>
@@ -11070,7 +11070,7 @@
       <c r="V23" s="144"/>
       <c r="W23" s="143">
         <f t="shared" ca="1" si="0"/>
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="X23" s="144">
         <v>72686</v>
@@ -11148,7 +11148,7 @@
       <c r="V24" s="149"/>
       <c r="W24" s="148">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="X24" s="149">
         <v>43374</v>
@@ -11310,7 +11310,7 @@
       <c r="V26" s="159"/>
       <c r="W26" s="158">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="X26" s="159">
         <v>72686</v>
@@ -11390,7 +11390,7 @@
       <c r="V27" s="164"/>
       <c r="W27" s="163">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="X27" s="164">
         <v>43451</v>
@@ -11468,7 +11468,7 @@
       <c r="V28" s="169"/>
       <c r="W28" s="168">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="X28" s="169">
         <v>72686</v>
@@ -11548,7 +11548,7 @@
       <c r="V29" s="174"/>
       <c r="W29" s="173">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="X29" s="174">
         <v>72686</v>
@@ -11628,7 +11628,7 @@
       <c r="V30" s="179"/>
       <c r="W30" s="178">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="X30" s="179">
         <v>43402</v>
@@ -11706,7 +11706,7 @@
       <c r="V31" s="184"/>
       <c r="W31" s="183">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="X31" s="184">
         <v>43451</v>
@@ -11786,7 +11786,7 @@
       <c r="V32" s="189"/>
       <c r="W32" s="188">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="X32" s="189">
         <v>43451</v>
@@ -11864,7 +11864,7 @@
       <c r="V33" s="194"/>
       <c r="W33" s="193">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X33" s="194">
         <v>72686</v>
@@ -11942,7 +11942,7 @@
       <c r="V34" s="199"/>
       <c r="W34" s="198">
         <f t="shared" ref="W34:W65" ca="1" si="1">IF(S34 = "", "", IF( V34 = "", TODAY() - S34, V34 - S34 ))</f>
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="X34" s="199">
         <v>72686</v>
@@ -12022,7 +12022,7 @@
       <c r="V35" s="204"/>
       <c r="W35" s="203">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="X35" s="204">
         <v>72686</v>
@@ -12100,7 +12100,7 @@
       <c r="V36" s="209"/>
       <c r="W36" s="208">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="X36" s="209">
         <v>72686</v>
@@ -12252,7 +12252,7 @@
       <c r="V38" s="218"/>
       <c r="W38" s="217">
         <f t="shared" ca="1" si="1"/>
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="X38" s="218">
         <v>43255</v>
@@ -12330,7 +12330,7 @@
       <c r="V39" s="223"/>
       <c r="W39" s="222">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="X39" s="223">
         <v>72686</v>
@@ -12488,7 +12488,7 @@
       <c r="V41" s="233"/>
       <c r="W41" s="232">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X41" s="233"/>
       <c r="Y41" s="231" t="s">
@@ -12564,7 +12564,7 @@
       <c r="V42" s="238"/>
       <c r="W42" s="237">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X42" s="238"/>
       <c r="Y42" s="236" t="s">
@@ -12640,7 +12640,7 @@
       <c r="V43" s="243"/>
       <c r="W43" s="242">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X43" s="243"/>
       <c r="Y43" s="241" t="s">
@@ -12716,7 +12716,7 @@
       <c r="V44" s="248"/>
       <c r="W44" s="247">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X44" s="248"/>
       <c r="Y44" s="246" t="s">
@@ -12792,7 +12792,7 @@
       <c r="V45" s="253"/>
       <c r="W45" s="252">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X45" s="253"/>
       <c r="Y45" s="251" t="s">
@@ -12868,7 +12868,7 @@
       <c r="V46" s="258"/>
       <c r="W46" s="257">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X46" s="258"/>
       <c r="Y46" s="256" t="s">
@@ -12944,7 +12944,7 @@
       <c r="V47" s="263"/>
       <c r="W47" s="262">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X47" s="263"/>
       <c r="Y47" s="261" t="s">
@@ -13020,7 +13020,7 @@
       <c r="V48" s="268"/>
       <c r="W48" s="267">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X48" s="268"/>
       <c r="Y48" s="266" t="s">
@@ -13096,7 +13096,7 @@
       <c r="V49" s="273"/>
       <c r="W49" s="272">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X49" s="273"/>
       <c r="Y49" s="271" t="s">
@@ -13172,7 +13172,7 @@
       <c r="V50" s="278"/>
       <c r="W50" s="277">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X50" s="278"/>
       <c r="Y50" s="276" t="s">
@@ -13248,7 +13248,7 @@
       <c r="V51" s="283"/>
       <c r="W51" s="282">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X51" s="283"/>
       <c r="Y51" s="281" t="s">
@@ -13324,7 +13324,7 @@
       <c r="V52" s="288"/>
       <c r="W52" s="287">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X52" s="288"/>
       <c r="Y52" s="286" t="s">
@@ -13400,7 +13400,7 @@
       <c r="V53" s="293"/>
       <c r="W53" s="292">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X53" s="293"/>
       <c r="Y53" s="291" t="s">
@@ -13476,7 +13476,7 @@
       <c r="V54" s="298"/>
       <c r="W54" s="297">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X54" s="298"/>
       <c r="Y54" s="296" t="s">
@@ -13552,7 +13552,7 @@
       <c r="V55" s="303"/>
       <c r="W55" s="302">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X55" s="303"/>
       <c r="Y55" s="301" t="s">
@@ -13628,7 +13628,7 @@
       <c r="V56" s="308"/>
       <c r="W56" s="307">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X56" s="308"/>
       <c r="Y56" s="306" t="s">
@@ -13704,7 +13704,7 @@
       <c r="V57" s="313"/>
       <c r="W57" s="312">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X57" s="313"/>
       <c r="Y57" s="311" t="s">
@@ -13780,7 +13780,7 @@
       <c r="V58" s="318"/>
       <c r="W58" s="317">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X58" s="318">
         <v>43416</v>
@@ -13858,7 +13858,7 @@
       <c r="V59" s="323"/>
       <c r="W59" s="322">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X59" s="323"/>
       <c r="Y59" s="321" t="s">
@@ -13934,7 +13934,7 @@
       <c r="V60" s="328"/>
       <c r="W60" s="327">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X60" s="328"/>
       <c r="Y60" s="326" t="s">
@@ -14010,7 +14010,7 @@
       <c r="V61" s="333"/>
       <c r="W61" s="332">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X61" s="333"/>
       <c r="Y61" s="331" t="s">
@@ -14086,7 +14086,7 @@
       <c r="V62" s="338"/>
       <c r="W62" s="337">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X62" s="338"/>
       <c r="Y62" s="336" t="s">
@@ -14162,7 +14162,7 @@
       <c r="V63" s="343"/>
       <c r="W63" s="342">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X63" s="343"/>
       <c r="Y63" s="341" t="s">
@@ -14238,7 +14238,7 @@
       <c r="V64" s="348"/>
       <c r="W64" s="347">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="X64" s="348"/>
       <c r="Y64" s="346" t="s">
@@ -14316,7 +14316,7 @@
       <c r="V65" s="353"/>
       <c r="W65" s="352">
         <f t="shared" ca="1" si="1"/>
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="X65" s="353">
         <v>43255</v>
@@ -14396,7 +14396,7 @@
       <c r="V66" s="358"/>
       <c r="W66" s="357">
         <f t="shared" ref="W66:W97" ca="1" si="2">IF(S66 = "", "", IF( V66 = "", TODAY() - S66, V66 - S66 ))</f>
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="X66" s="358">
         <v>43416</v>
@@ -14474,7 +14474,7 @@
       <c r="V67" s="363"/>
       <c r="W67" s="362">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X67" s="363"/>
       <c r="Y67" s="361" t="s">
@@ -14552,7 +14552,7 @@
       <c r="V68" s="368"/>
       <c r="W68" s="367">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="X68" s="368">
         <v>43451</v>
@@ -14630,7 +14630,7 @@
       <c r="V69" s="373"/>
       <c r="W69" s="372">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X69" s="373"/>
       <c r="Y69" s="371" t="s">
@@ -14708,7 +14708,7 @@
       <c r="V70" s="378"/>
       <c r="W70" s="377">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="X70" s="378">
         <v>43451</v>
@@ -14786,7 +14786,7 @@
       <c r="V71" s="383"/>
       <c r="W71" s="382">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X71" s="383"/>
       <c r="Y71" s="381" t="s">
@@ -14862,7 +14862,7 @@
       <c r="V72" s="388"/>
       <c r="W72" s="387">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="X72" s="388">
         <v>43451</v>
@@ -14940,7 +14940,7 @@
       <c r="V73" s="393"/>
       <c r="W73" s="392">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X73" s="393"/>
       <c r="Y73" s="391" t="s">
@@ -15016,7 +15016,7 @@
       <c r="V74" s="398"/>
       <c r="W74" s="397">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="X74" s="398">
         <v>43451</v>
@@ -15094,7 +15094,7 @@
       <c r="V75" s="403"/>
       <c r="W75" s="402">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="X75" s="403">
         <v>43451</v>
@@ -15174,7 +15174,7 @@
       <c r="V76" s="408"/>
       <c r="W76" s="407">
         <f t="shared" ca="1" si="2"/>
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="X76" s="408">
         <v>43213</v>
@@ -15326,7 +15326,7 @@
       <c r="V78" s="417"/>
       <c r="W78" s="416">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="X78" s="417">
         <v>72686</v>
@@ -15406,7 +15406,7 @@
       <c r="V79" s="422"/>
       <c r="W79" s="421">
         <f t="shared" ca="1" si="2"/>
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="X79" s="422">
         <v>72686</v>
@@ -15484,7 +15484,7 @@
       <c r="V80" s="427"/>
       <c r="W80" s="426">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="X80" s="427">
         <v>72686</v>
@@ -15562,7 +15562,7 @@
       <c r="V81" s="432"/>
       <c r="W81" s="431">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="X81" s="432">
         <v>72686</v>
@@ -15640,7 +15640,7 @@
       <c r="V82" s="437"/>
       <c r="W82" s="436">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X82" s="437"/>
       <c r="Y82" s="435" t="s">
@@ -15716,7 +15716,7 @@
       <c r="V83" s="442"/>
       <c r="W83" s="441">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="X83" s="442">
         <v>72686</v>
@@ -15864,7 +15864,7 @@
       <c r="V85" s="451"/>
       <c r="W85" s="450">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X85" s="451">
         <v>43451</v>
@@ -15942,7 +15942,7 @@
       <c r="V86" s="456"/>
       <c r="W86" s="455">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X86" s="456">
         <v>43451</v>
@@ -16020,7 +16020,7 @@
       <c r="V87" s="461"/>
       <c r="W87" s="460">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="X87" s="461">
         <v>72686</v>
@@ -16098,7 +16098,7 @@
       <c r="V88" s="466"/>
       <c r="W88" s="465">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="X88" s="466">
         <v>72686</v>
@@ -16176,7 +16176,7 @@
       <c r="V89" s="471"/>
       <c r="W89" s="470">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X89" s="471">
         <v>43606</v>
@@ -16254,7 +16254,7 @@
       <c r="V90" s="476"/>
       <c r="W90" s="475">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X90" s="476">
         <v>72686</v>
@@ -16332,7 +16332,7 @@
       <c r="V91" s="481"/>
       <c r="W91" s="480">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X91" s="481">
         <v>72686</v>
@@ -16410,7 +16410,7 @@
       <c r="V92" s="486"/>
       <c r="W92" s="485">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X92" s="486">
         <v>72686</v>
@@ -16558,7 +16558,7 @@
       <c r="V94" s="495"/>
       <c r="W94" s="494">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X94" s="495">
         <v>72686</v>
@@ -16706,7 +16706,7 @@
       <c r="V96" s="504"/>
       <c r="W96" s="503">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X96" s="504"/>
       <c r="Y96" s="502" t="s">
@@ -16782,7 +16782,7 @@
       <c r="V97" s="509"/>
       <c r="W97" s="508">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X97" s="509">
         <v>43451</v>
@@ -16855,7 +16855,7 @@
       <c r="U98" s="514"/>
       <c r="V98" s="514"/>
       <c r="W98" s="513" t="str">
-        <f t="shared" ref="W98:W129" ca="1" si="3">IF(S98 = "", "", IF( V98 = "", TODAY() - S98, V98 - S98 ))</f>
+        <f t="shared" ref="W98:W105" ca="1" si="3">IF(S98 = "", "", IF( V98 = "", TODAY() - S98, V98 - S98 ))</f>
         <v/>
       </c>
       <c r="X98" s="514">
@@ -16934,7 +16934,7 @@
       <c r="V99" s="518"/>
       <c r="W99" s="517">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="X99" s="518">
         <v>43501</v>
@@ -17012,7 +17012,7 @@
       <c r="V100" s="523"/>
       <c r="W100" s="522">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="X100" s="523">
         <v>43451</v>
@@ -17608,6 +17608,7 @@
     <hyperlink ref="I105" r:id="rId196"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId197"/>
 </worksheet>
 </file>
 

</xml_diff>